<commit_message>
A Sept 20 commit
</commit_message>
<xml_diff>
--- a/latex/wp1/Russia r S.xlsx
+++ b/latex/wp1/Russia r S.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harry\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Country\Russia\Data\SEASHELL\SEABYTE\edreru\latex\wp1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FA92A25-BB12-43ED-9C69-81B21ADA38C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD7EAAD-3429-44AA-9125-37B8146E1314}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" xr2:uid="{3DDFCE6F-82E4-47C7-8EA5-9DA5FC3EC93F}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="23040" windowHeight="12204" xr2:uid="{3DDFCE6F-82E4-47C7-8EA5-9DA5FC3EC93F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -49,7 +47,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -94,7 +92,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -102,11 +100,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -494,31 +489,31 @@
             <c:numRef>
               <c:f>Sheet1!$C$2:$C$26</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
+                  <c:v>7.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>8.4</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7.1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.8000000000000007</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.6999999999999993</c:v>
+                  <c:v>8.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.3000000000000007</c:v>
+                  <c:v>9.1999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.1999999999999993</c:v>
+                  <c:v>9.1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.3000000000000007</c:v>
+                  <c:v>9.1</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>8.5</c:v>
@@ -527,22 +522,22 @@
                   <c:v>8.1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8</c:v>
+                  <c:v>8.1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.6</c:v>
+                  <c:v>6.4</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>7.9</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7.6</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.1</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.7</c:v>
+                  <c:v>6.6</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>6.1</c:v>
@@ -560,7 +555,7 @@
                   <c:v>6.1</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5.4</c:v>
+                  <c:v>5.3</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>5.4</c:v>
@@ -695,7 +690,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -748,6 +743,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="596225568"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1384,13 +1380,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
@@ -1721,7 +1717,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1730,13 +1726,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1747,8 +1743,8 @@
       <c r="B2" s="3">
         <v>12.7</v>
       </c>
-      <c r="C2" s="4">
-        <v>8.4</v>
+      <c r="C2">
+        <v>7.3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1758,8 +1754,8 @@
       <c r="B3" s="3">
         <v>12.7</v>
       </c>
-      <c r="C3" s="4">
-        <v>7.8</v>
+      <c r="C3">
+        <v>7.6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1769,8 +1765,8 @@
       <c r="B4" s="3">
         <v>12.8</v>
       </c>
-      <c r="C4" s="4">
-        <v>7.1</v>
+      <c r="C4">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1780,8 +1776,8 @@
       <c r="B5" s="3">
         <v>12.7</v>
       </c>
-      <c r="C5" s="4">
-        <v>8.8000000000000007</v>
+      <c r="C5">
+        <v>8.4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1791,8 +1787,8 @@
       <c r="B6" s="3">
         <v>12.7</v>
       </c>
-      <c r="C6" s="4">
-        <v>8.6999999999999993</v>
+      <c r="C6">
+        <v>8.4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1802,8 +1798,8 @@
       <c r="B7" s="3">
         <v>12.8</v>
       </c>
-      <c r="C7" s="4">
-        <v>9.3000000000000007</v>
+      <c r="C7">
+        <v>9.1999999999999993</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1813,8 +1809,8 @@
       <c r="B8" s="3">
         <v>12.8</v>
       </c>
-      <c r="C8" s="4">
-        <v>9.1999999999999993</v>
+      <c r="C8">
+        <v>9.1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1824,8 +1820,8 @@
       <c r="B9" s="3">
         <v>12.8</v>
       </c>
-      <c r="C9" s="4">
-        <v>9.3000000000000007</v>
+      <c r="C9">
+        <v>9.1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1835,7 +1831,7 @@
       <c r="B10" s="3">
         <v>12.8</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10">
         <v>8.5</v>
       </c>
     </row>
@@ -1846,7 +1842,7 @@
       <c r="B11" s="3">
         <v>12.8</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11">
         <v>8.1</v>
       </c>
     </row>
@@ -1857,8 +1853,8 @@
       <c r="B12" s="3">
         <v>12.8</v>
       </c>
-      <c r="C12" s="4">
-        <v>8</v>
+      <c r="C12">
+        <v>8.1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1868,8 +1864,8 @@
       <c r="B13" s="3">
         <v>12.8</v>
       </c>
-      <c r="C13" s="4">
-        <v>6.6</v>
+      <c r="C13">
+        <v>6.4</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1879,7 +1875,7 @@
       <c r="B14" s="3">
         <v>12.9</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14">
         <v>7.9</v>
       </c>
     </row>
@@ -1890,8 +1886,8 @@
       <c r="B15" s="3">
         <v>12.9</v>
       </c>
-      <c r="C15" s="4">
-        <v>7.6</v>
+      <c r="C15">
+        <v>7.5</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -1901,8 +1897,8 @@
       <c r="B16" s="3">
         <v>13</v>
       </c>
-      <c r="C16" s="4">
-        <v>7.1</v>
+      <c r="C16">
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -1912,8 +1908,8 @@
       <c r="B17" s="3">
         <v>13</v>
       </c>
-      <c r="C17" s="4">
-        <v>6.7</v>
+      <c r="C17">
+        <v>6.6</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -1923,7 +1919,7 @@
       <c r="B18" s="3">
         <v>13</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18">
         <v>6.1</v>
       </c>
     </row>
@@ -1934,7 +1930,7 @@
       <c r="B19" s="3">
         <v>13.1</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19">
         <v>6.5</v>
       </c>
     </row>
@@ -1945,7 +1941,7 @@
       <c r="B20" s="3">
         <v>13.1</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20">
         <v>6.8</v>
       </c>
     </row>
@@ -1956,7 +1952,7 @@
       <c r="B21" s="3">
         <v>13.2</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21">
         <v>5.7</v>
       </c>
     </row>
@@ -1967,7 +1963,7 @@
       <c r="B22" s="3">
         <v>13.3</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22">
         <v>6.1</v>
       </c>
     </row>
@@ -1978,8 +1974,8 @@
       <c r="B23" s="3">
         <v>13.3</v>
       </c>
-      <c r="C23" s="4">
-        <v>5.4</v>
+      <c r="C23">
+        <v>5.3</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -1989,12 +1985,13 @@
       <c r="B24" s="3">
         <v>13.3</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24">
         <v>5.4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>